<commit_message>
chp technology implementation - available fuel feature
</commit_message>
<xml_diff>
--- a/techs/chp_maps/CHPmaps.xlsx
+++ b/techs/chp_maps/CHPmaps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mati\documenti\GitHub\MESSpy\techs\chp_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C043D09A-148C-4273-B307-CA3EF72F2BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034F7C91-5486-4C7A-B61B-5F1428114ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15480" yWindow="4575" windowWidth="15600" windowHeight="11160" xr2:uid="{FB6132EF-F7C4-4AEF-BAC3-B19BC1648422}"/>
+    <workbookView xWindow="-15480" yWindow="4575" windowWidth="15600" windowHeight="11160" activeTab="3" xr2:uid="{FB6132EF-F7C4-4AEF-BAC3-B19BC1648422}"/>
   </bookViews>
   <sheets>
     <sheet name="m_steam" sheetId="1" r:id="rId1"/>
@@ -119,10 +119,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F68191-AC1D-4D9C-9040-D8E3ADDD8166}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:K20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,15 +451,15 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -681,7 +681,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB99C56-A0B1-4AAC-8996-2838DB548C77}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -691,15 +693,15 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -732,8 +734,7 @@
         <v>-10</v>
       </c>
       <c r="B4">
-        <f>C4-700</f>
-        <v>2316.4699999999998</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>3016.47</v>
@@ -759,8 +760,7 @@
         <v>0</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:B10" si="0">C5-700</f>
-        <v>1928.46</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>2628.46</v>
@@ -786,8 +786,7 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
-        <v>1587.94</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>2287.94</v>
@@ -813,8 +812,7 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
-        <v>1433.3400000000001</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>2133.34</v>
@@ -840,8 +838,7 @@
         <v>20</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
-        <v>1287.96</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>1987.96</v>
@@ -867,8 +864,7 @@
         <v>30</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
-        <v>1021.6800000000001</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <v>1721.68</v>
@@ -894,8 +890,7 @@
         <v>40</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
-        <v>784.69</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <v>1484.69</v>
@@ -928,7 +923,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC92FD78-6735-4B79-AEDD-ACDEEA834CD8}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -938,15 +935,15 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -979,8 +976,7 @@
         <v>-10</v>
       </c>
       <c r="B4">
-        <f>C4-2100</f>
-        <v>6949.41</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>9049.41</v>
@@ -1006,8 +1002,7 @@
         <v>0</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:B10" si="0">C5-2100</f>
-        <v>5785.38</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>7885.38</v>
@@ -1033,8 +1028,7 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
-        <v>4763.82</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>6863.82</v>
@@ -1060,8 +1054,7 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
-        <v>4300.0200000000004</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>6400.02</v>
@@ -1087,8 +1080,7 @@
         <v>20</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
-        <v>3863.88</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>5963.88</v>
@@ -1114,8 +1106,7 @@
         <v>30</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
-        <v>3065.04</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <v>5165.04</v>
@@ -1141,8 +1132,7 @@
         <v>40</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
-        <v>2354.0699999999997</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <v>4454.07</v>
@@ -1175,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0DDE5BE-2339-45B5-98F7-1DF779621358}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1187,15 +1177,15 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1228,7 +1218,7 @@
         <v>-10</v>
       </c>
       <c r="B4">
-        <v>344.88</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>344.88</v>
@@ -1254,7 +1244,7 @@
         <v>0</v>
       </c>
       <c r="B5">
-        <v>317.15999999999997</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>317.15999999999997</v>
@@ -1280,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>292.68</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>292.68</v>
@@ -1306,7 +1296,7 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>281.16000000000003</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>281.16000000000003</v>
@@ -1332,7 +1322,7 @@
         <v>20</v>
       </c>
       <c r="B8">
-        <v>270.36</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>270.36</v>
@@ -1358,7 +1348,7 @@
         <v>30</v>
       </c>
       <c r="B9">
-        <v>249.84</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <v>249.84</v>
@@ -1384,7 +1374,7 @@
         <v>40</v>
       </c>
       <c r="B10">
-        <v>231.48</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <v>231.48</v>
@@ -1406,67 +1396,67 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1481,7 +1471,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B241F22-E11B-4901-9BF2-3399D531A86E}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1491,15 +1483,15 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1532,7 +1524,7 @@
         <v>-10</v>
       </c>
       <c r="B4">
-        <v>1133.6849999999999</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>1133.6849999999999</v>
@@ -1558,7 +1550,7 @@
         <v>0</v>
       </c>
       <c r="B5">
-        <v>1129.8820000000001</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>1129.8820000000001</v>
@@ -1584,7 +1576,7 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>1126.7370000000001</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>1126.7370000000001</v>
@@ -1610,7 +1602,7 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>1125.4059999999999</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>1125.4059999999999</v>
@@ -1636,7 +1628,7 @@
         <v>20</v>
       </c>
       <c r="B8">
-        <v>1124.2170000000001</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>1124.2170000000001</v>
@@ -1662,7 +1654,7 @@
         <v>30</v>
       </c>
       <c r="B9">
-        <v>1122.309</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <v>1122.309</v>
@@ -1688,7 +1680,7 @@
         <v>40</v>
       </c>
       <c r="B10">
-        <v>1121.009</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <v>1121.009</v>
@@ -1725,7 +1717,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FF277A-01C6-404B-ACFC-45A27A6D73E8}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1735,15 +1729,15 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
minor bugs fixed on CHP
</commit_message>
<xml_diff>
--- a/techs/chp_maps/CHPmaps.xlsx
+++ b/techs/chp_maps/CHPmaps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mati\documenti\GitHub\MESSpy\techs\chp_maps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calabresi\Desktop\Dottorato\Git_MESS\MESSpy\techs\chp_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034F7C91-5486-4C7A-B61B-5F1428114ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65098E9E-B29F-48C7-85D8-AE437394BB48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15480" yWindow="4575" windowWidth="15600" windowHeight="11160" activeTab="3" xr2:uid="{FB6132EF-F7C4-4AEF-BAC3-B19BC1648422}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{FB6132EF-F7C4-4AEF-BAC3-B19BC1648422}"/>
   </bookViews>
   <sheets>
     <sheet name="m_steam" sheetId="1" r:id="rId1"/>
@@ -49,22 +49,22 @@
     <t>Load [-](mvap%)</t>
   </si>
   <si>
-    <t>m steam [kg/h]</t>
-  </si>
-  <si>
     <t>W el  [kW]</t>
   </si>
   <si>
     <t>Q th [kW]</t>
   </si>
   <si>
-    <t>m fuel [kg/h]</t>
-  </si>
-  <si>
     <t>TIT [K]</t>
   </si>
   <si>
     <t>T stack [K]</t>
+  </si>
+  <si>
+    <t>m steam [kg/s]</t>
+  </si>
+  <si>
+    <t>m fuel [kg/s]</t>
   </si>
 </sst>
 </file>
@@ -141,9 +141,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -181,7 +181,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -287,7 +287,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -429,7 +429,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -440,14 +440,14 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -495,22 +495,22 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>5400</v>
+        <v>1.5</v>
       </c>
       <c r="D4">
-        <v>7200</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>10800</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>14400</v>
+        <v>4</v>
       </c>
       <c r="G4">
-        <v>18000</v>
+        <v>5</v>
       </c>
       <c r="H4">
-        <v>21600</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -521,22 +521,22 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>5400</v>
+        <v>1.5</v>
       </c>
       <c r="D5">
-        <v>7200</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>10800</v>
+        <v>3</v>
       </c>
       <c r="F5">
-        <v>14400</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>18000</v>
+        <v>5</v>
       </c>
       <c r="H5">
-        <v>21600</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -547,22 +547,22 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>5400</v>
+        <v>1.5</v>
       </c>
       <c r="D6">
-        <v>7200</v>
+        <v>2</v>
       </c>
       <c r="E6">
-        <v>10800</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>14400</v>
+        <v>4</v>
       </c>
       <c r="G6">
-        <v>18000</v>
+        <v>5</v>
       </c>
       <c r="H6">
-        <v>21600</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -573,22 +573,22 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>5400</v>
+        <v>1.5</v>
       </c>
       <c r="D7">
-        <v>7200</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>10800</v>
+        <v>3</v>
       </c>
       <c r="F7">
-        <v>14400</v>
+        <v>4</v>
       </c>
       <c r="G7">
-        <v>18000</v>
+        <v>5</v>
       </c>
       <c r="H7">
-        <v>21600</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -599,22 +599,22 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>5400</v>
+        <v>1.5</v>
       </c>
       <c r="D8">
-        <v>7200</v>
+        <v>2</v>
       </c>
       <c r="E8">
-        <v>10800</v>
+        <v>3</v>
       </c>
       <c r="F8">
-        <v>14400</v>
+        <v>4</v>
       </c>
       <c r="G8">
-        <v>18000</v>
+        <v>5</v>
       </c>
       <c r="H8">
-        <v>21600</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -625,22 +625,22 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>5400</v>
+        <v>1.5</v>
       </c>
       <c r="D9">
-        <v>7200</v>
+        <v>2</v>
       </c>
       <c r="E9">
-        <v>10800</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>14400</v>
+        <v>4</v>
       </c>
       <c r="G9">
-        <v>18000</v>
+        <v>5</v>
       </c>
       <c r="H9">
-        <v>21600</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -651,22 +651,22 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>5400</v>
+        <v>1.5</v>
       </c>
       <c r="D10">
-        <v>7200</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>10800</v>
+        <v>3</v>
       </c>
       <c r="F10">
-        <v>14400</v>
+        <v>4</v>
       </c>
       <c r="G10">
-        <v>18000</v>
+        <v>5</v>
       </c>
       <c r="H10">
-        <v>21600</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -689,7 +689,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -931,7 +931,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1166,14 +1166,14 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="J4" sqref="J4:O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1221,22 +1221,22 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>344.88</v>
+        <v>9.5799999999999996E-2</v>
       </c>
       <c r="D4">
-        <v>396.72</v>
+        <v>0.11020000000000001</v>
       </c>
       <c r="E4">
-        <v>498.96</v>
+        <v>0.1386</v>
       </c>
       <c r="F4">
-        <v>607.31999999999994</v>
+        <v>0.16869999999999999</v>
       </c>
       <c r="G4">
-        <v>721.43999999999994</v>
+        <v>0.20039999999999999</v>
       </c>
       <c r="H4">
-        <v>839.88</v>
+        <v>0.23330000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1247,22 +1247,22 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>317.15999999999997</v>
+        <v>8.8099999999999998E-2</v>
       </c>
       <c r="D5">
-        <v>368.28000000000003</v>
+        <v>0.1023</v>
       </c>
       <c r="E5">
-        <v>470.15999999999997</v>
+        <v>0.13059999999999999</v>
       </c>
       <c r="F5">
-        <v>578.88</v>
+        <v>0.1608</v>
       </c>
       <c r="G5">
-        <v>693.72</v>
+        <v>0.19270000000000001</v>
       </c>
       <c r="H5">
-        <v>812.16</v>
+        <v>0.22559999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1273,22 +1273,22 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>292.68</v>
+        <v>8.1299999999999997E-2</v>
       </c>
       <c r="D6">
-        <v>343.08</v>
+        <v>9.5299999999999996E-2</v>
       </c>
       <c r="E6">
-        <v>444.96</v>
+        <v>0.12359999999999999</v>
       </c>
       <c r="F6">
-        <v>553.67999999999995</v>
+        <v>0.15379999999999999</v>
       </c>
       <c r="G6">
-        <v>668.52</v>
+        <v>0.1857</v>
       </c>
       <c r="H6">
-        <v>787.32</v>
+        <v>0.21870000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1299,22 +1299,22 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>281.16000000000003</v>
+        <v>7.8100000000000003E-2</v>
       </c>
       <c r="D7">
-        <v>331.2</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="E7">
-        <v>433.08000000000004</v>
+        <v>0.12030000000000002</v>
       </c>
       <c r="F7">
-        <v>542.16000000000008</v>
+        <v>0.15060000000000001</v>
       </c>
       <c r="G7">
-        <v>657.36</v>
+        <v>0.18260000000000001</v>
       </c>
       <c r="H7">
-        <v>775.8</v>
+        <v>0.2155</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1325,22 +1325,22 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>270.36</v>
+        <v>7.51E-2</v>
       </c>
       <c r="D8">
-        <v>320.04000000000002</v>
+        <v>8.8900000000000007E-2</v>
       </c>
       <c r="E8">
-        <v>421.92</v>
+        <v>0.1172</v>
       </c>
       <c r="F8">
-        <v>531</v>
+        <v>0.14749999999999999</v>
       </c>
       <c r="G8">
-        <v>646.19999999999993</v>
+        <v>0.17949999999999999</v>
       </c>
       <c r="H8">
-        <v>764.64</v>
+        <v>0.21240000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1351,22 +1351,22 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>249.84</v>
+        <v>6.9400000000000003E-2</v>
       </c>
       <c r="D9">
-        <v>299.52</v>
+        <v>8.3199999999999996E-2</v>
       </c>
       <c r="E9">
-        <v>401.04</v>
+        <v>0.1114</v>
       </c>
       <c r="F9">
-        <v>510.48</v>
+        <v>0.14180000000000001</v>
       </c>
       <c r="G9">
-        <v>626.04</v>
+        <v>0.1739</v>
       </c>
       <c r="H9">
-        <v>744.48</v>
+        <v>0.20680000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1377,22 +1377,22 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>231.48</v>
+        <v>6.4299999999999996E-2</v>
       </c>
       <c r="D10">
-        <v>280.44</v>
+        <v>7.7899999999999997E-2</v>
       </c>
       <c r="E10">
-        <v>382.32</v>
+        <v>0.1062</v>
       </c>
       <c r="F10">
-        <v>492.11999999999995</v>
+        <v>0.13669999999999999</v>
       </c>
       <c r="G10">
-        <v>607.68000000000006</v>
+        <v>0.16880000000000001</v>
       </c>
       <c r="H10">
-        <v>725.76</v>
+        <v>0.2016</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1479,7 +1479,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1725,7 +1725,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>